<commit_message>
Plusieurs fomat de clefs crees
Rajouter authentication en lisant read me et faire fonctionner ce truc a la maison
</commit_message>
<xml_diff>
--- a/Cahier des charges/READ ME.xlsx
+++ b/Cahier des charges/READ ME.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAC0BEBB-2EF2-48F3-BE2C-F5DDEFE81236}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671A9B36-EE51-4E01-A09C-5852426DD6BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="2" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ports" sheetId="1" r:id="rId1"/>
+    <sheet name="authentication db info" sheetId="2" r:id="rId2"/>
+    <sheet name="Comment gerer les jwt" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t>Recap des ports used dans les applis node.js</t>
     <phoneticPr fontId="1"/>
@@ -61,6 +63,409 @@
   </si>
   <si>
     <t>Server qui permet de modifier les comptes d'access token</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>action</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mongo/authentication</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mongo/graph-*</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mysql/bejewel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mysql/ogor.io</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>issuer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>kevin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>login</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>audience</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>createdAt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>updatedAt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>P!Auronlegris1P</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jwt_admin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>expireAt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1d</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jwt_mng</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_graph</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_Bejewel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Wistala91</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bejewel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>game1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_ogor.ia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>123S0L3I</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ogor.ia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>game2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_rest_db_conn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>igcwCZ6U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dbRequestServer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fastDbReq</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>db1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>db2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>db3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>r/rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mongo/CRUD-MYSQL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mysql/crud_mysql</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>server</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>localhost:3004</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>localhost:3001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まだ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>localhost:3002</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>30m</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1m</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>icon</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>m2Psg1s!Xw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{2!dGcA9ljk</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{+cSe1sAx</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>p2C6xui3Ds0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>x7SaF}o0lI1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_admin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>graph_api</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>live_info</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>QoiVyjO6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5a408a13b2bc34880b3934</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5a409d13b2bc34880b3935</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5a33a20c01273c68d078fd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5a405c13b2bc34880b3932</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5a407513b2bc34880b3933</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Modification des comptes de gestion des jwt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1 modifier la feuille de calcul : authentication db info</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2 Lancer une requete vers le server de generation des jwt et obtenir le jwt_admin account</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3 Utiliser ce jwt dans le systeme de securite et lancer la requete d'update/insert</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pour un insert il faut : name, login, password, audience, expiresIn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pour un update il faut au moins l'id recuperable dans mongodb</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pour proteger une page, ajouter dans le router du server correspondant les lignes suivantes :</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>const</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>validateToken</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>require</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'link_jwt'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>router</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFDCDCAA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>validateToken</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(audience_name))</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ou audience_name est le audience que vous avez insere/update</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -68,7 +473,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +498,84 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0451A5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDCDCAA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +618,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -320,13 +813,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -384,8 +964,102 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -973,14 +1647,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48162075-32B7-492A-BCCF-F27A03148D3E}">
-  <dimension ref="E2:G9"/>
+  <dimension ref="E2:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="66.125" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
@@ -998,7 +1673,9 @@
       <c r="F4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="5:7" ht="75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E5" s="4">
@@ -1044,6 +1721,93 @@
         <v>7</v>
       </c>
       <c r="G9" s="12"/>
+    </row>
+    <row r="15" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="5:7" x14ac:dyDescent="0.4">
+      <c r="F16" s="20"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F17" s="20"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F18" s="20"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F23" s="20"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F24" s="20"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F27" s="20"/>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F28" s="20"/>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F29" s="20"/>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F31" s="19"/>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F32" s="20"/>
+    </row>
+    <row r="33" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="F34" s="20"/>
+    </row>
+    <row r="35" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="F35" s="19"/>
+    </row>
+    <row r="37" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="T37" s="21"/>
+    </row>
+    <row r="38" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="T38" s="21"/>
+    </row>
+    <row r="39" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="T39" s="21"/>
+    </row>
+    <row r="40" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="T40" s="21"/>
+    </row>
+    <row r="42" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="T42" s="21"/>
+    </row>
+    <row r="43" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="T43" s="21"/>
+    </row>
+    <row r="44" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="T44" s="21"/>
+    </row>
+    <row r="45" spans="6:20" x14ac:dyDescent="0.4">
+      <c r="T45" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1051,4 +1815,440 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1AC559-EAEB-434C-971F-21A81182D7FD}">
+  <dimension ref="A1:Q38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="9" style="22"/>
+    <col min="2" max="2" width="32.75" style="22" customWidth="1"/>
+    <col min="3" max="3" width="15.625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="16.25" style="22" customWidth="1"/>
+    <col min="6" max="6" width="15" style="22" customWidth="1"/>
+    <col min="7" max="9" width="11.375" style="22" customWidth="1"/>
+    <col min="10" max="10" width="9" style="22"/>
+    <col min="11" max="11" width="18.5" style="22" customWidth="1"/>
+    <col min="12" max="12" width="19.375" style="22" customWidth="1"/>
+    <col min="13" max="13" width="20.375" style="22" customWidth="1"/>
+    <col min="14" max="14" width="9" style="22"/>
+    <col min="15" max="15" width="25.75" style="22" customWidth="1"/>
+    <col min="16" max="16" width="16.875" style="22" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="40">
+        <v>43696</v>
+      </c>
+      <c r="J3" s="40">
+        <v>43696</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="25">
+        <v>43696</v>
+      </c>
+      <c r="J4" s="25">
+        <v>43696</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="36">
+        <v>43696</v>
+      </c>
+      <c r="J5" s="36">
+        <v>43696</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="36">
+        <v>43696</v>
+      </c>
+      <c r="J6" s="36">
+        <v>43696</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6" s="37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="32">
+        <v>43696</v>
+      </c>
+      <c r="J7" s="32">
+        <v>43696</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q14" s="23"/>
+    </row>
+    <row r="15" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q15" s="23"/>
+    </row>
+    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q16" s="23"/>
+    </row>
+    <row r="17" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q17" s="23"/>
+    </row>
+    <row r="19" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q19" s="23"/>
+    </row>
+    <row r="20" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q20" s="23"/>
+    </row>
+    <row r="21" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q21" s="23"/>
+    </row>
+    <row r="22" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q22" s="23"/>
+    </row>
+    <row r="30" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O30" s="23"/>
+    </row>
+    <row r="31" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O31" s="23"/>
+    </row>
+    <row r="32" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O32" s="23"/>
+    </row>
+    <row r="33" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O33" s="23"/>
+    </row>
+    <row r="35" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O35" s="23"/>
+    </row>
+    <row r="36" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O36" s="23"/>
+    </row>
+    <row r="37" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O37" s="23"/>
+    </row>
+    <row r="38" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="O38" s="23"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EF3A77-BB80-4E84-8A01-F8C91F1840A5}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P23" sqref="P22:P23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B9" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B10" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de mongo db dans le gestionnaire de requet vers sgbd
</commit_message>
<xml_diff>
--- a/Cahier des charges/READ ME.xlsx
+++ b/Cahier des charges/READ ME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671A9B36-EE51-4E01-A09C-5852426DD6BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E18E16-BD25-4DEF-8E01-F3C0AC8E2D38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="2" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="1" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
   </bookViews>
   <sheets>
     <sheet name="ports" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="150">
   <si>
     <t>Recap des ports used dans les applis node.js</t>
     <phoneticPr fontId="1"/>
@@ -122,10 +122,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>P!Auronlegris1P</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>jwt_admin</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -150,10 +146,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Wistala91</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>bejewel</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -166,10 +158,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>123S0L3I</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ogor.ia</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -178,22 +166,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>KM_rest_db_conn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>igcwCZ6U</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dbRequestServer</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>fastDbReq</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>db1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -218,10 +190,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>r/rw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mongo/CRUD-MYSQL</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -262,26 +230,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>m2Psg1s!Xw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{2!dGcA9ljk</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{+cSe1sAx</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>p2C6xui3Ds0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>x7SaF}o0lI1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>KM_admin</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -291,26 +239,6 @@
   </si>
   <si>
     <t>live_info</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>QoiVyjO6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5a408a13b2bc34880b3934</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5a409d13b2bc34880b3935</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5a33a20c01273c68d078fd</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5a405c13b2bc34880b3932</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -468,12 +396,328 @@
     <t>ou audience_name est le audience que vous avez insere/update</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>r/rw</t>
+  </si>
+  <si>
+    <t>KM_db_c1r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c1rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c2r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c2rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c3r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c3rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c1w</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c2w</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c3w</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_db_c1r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_db_c1w</t>
+  </si>
+  <si>
+    <t>access_db_c1rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_c1r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_c1w</t>
+  </si>
+  <si>
+    <t>access_c1rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_c3w</t>
+  </si>
+  <si>
+    <t>access_c3rw</t>
+  </si>
+  <si>
+    <t>access_db_c2w</t>
+  </si>
+  <si>
+    <t>access_db_c2rw</t>
+  </si>
+  <si>
+    <t>access_db_c3w</t>
+  </si>
+  <si>
+    <t>access_db_c3rw</t>
+  </si>
+  <si>
+    <t>access_c2w</t>
+  </si>
+  <si>
+    <t>WQ?~&gt;R4z</t>
+  </si>
+  <si>
+    <t>%#n75kW%</t>
+  </si>
+  <si>
+    <t>9r%ANFhb</t>
+  </si>
+  <si>
+    <t>w4#7Ec$W</t>
+  </si>
+  <si>
+    <t>GYb!Q52E</t>
+  </si>
+  <si>
+    <t>xN!SJ26N</t>
+  </si>
+  <si>
+    <t>a%66#KFg</t>
+  </si>
+  <si>
+    <t>8P5!J#HL</t>
+  </si>
+  <si>
+    <t>&amp;MB3gZBS</t>
+  </si>
+  <si>
+    <t>+y&amp;WXY@2</t>
+  </si>
+  <si>
+    <t>LJN+Sb59</t>
+  </si>
+  <si>
+    <t>uWL845@#</t>
+  </si>
+  <si>
+    <t>fE&gt;a8Y3Q</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b88f2f3f2d3273ce26bcf</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8+N56?K&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b890ff3f2d3273ce26bd0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LFBa&amp;X8&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8934f3f2d3273ce26bd1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>t4N8b$Gc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b896ff3f2d3273ce26bd2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B4g+D85Q</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTRG%M68</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>!6Dq%h@u</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b89bcf3f2d3273ce26bd4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GaDS9?&amp;G</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8a1ff3f2d3273ce26bd5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_c2r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_db_c2r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8a40f3f2d3273ce26bd6</t>
+  </si>
+  <si>
+    <t>access_c2rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TC&amp;yJUy5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8adbf3f2d3273ce26bd7</t>
+  </si>
+  <si>
+    <t>nUT+Ds28</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8b0df3f2d3273ce26bd8</t>
+  </si>
+  <si>
+    <t>access_c3r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_db_c3r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>78B34B^Y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LHE?w4Tu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8b32f3f2d3273ce26bd9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>83Lt&amp;^44</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8b52f3f2d3273ce26bda</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8b69f3f2d3273ce26bdb</t>
+  </si>
+  <si>
+    <t>6+qx&gt;3R#</t>
+  </si>
+  <si>
+    <t>Q6G&amp;ntmJ</t>
+  </si>
+  <si>
+    <t>MXL8D?8k</t>
+  </si>
+  <si>
+    <t>KM_db_c0r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c0w</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KM_db_c0rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_c0r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_c0w</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_c0rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_db_c0r</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_db_c0w</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>access_db_c0rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Gf7@SEr7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>eD8D2Ty?</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8fa4a2a3ec5288524f8c</t>
+  </si>
+  <si>
+    <t>5d5b8fd1a2a3ec5288524f8d</t>
+  </si>
+  <si>
+    <t>UnpD$6CH</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5d5b8fe6a2a3ec5288524f8e</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,6 +818,18 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -906,7 +1162,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1055,6 +1311,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1674,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="5:7" ht="75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1819,33 +2096,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1AC559-EAEB-434C-971F-21A81182D7FD}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" style="22"/>
     <col min="2" max="2" width="32.75" style="22" customWidth="1"/>
-    <col min="3" max="3" width="15.625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="22" customWidth="1"/>
     <col min="4" max="4" width="15.125" style="22" customWidth="1"/>
     <col min="5" max="5" width="16.25" style="22" customWidth="1"/>
     <col min="6" max="6" width="15" style="22" customWidth="1"/>
     <col min="7" max="9" width="11.375" style="22" customWidth="1"/>
-    <col min="10" max="10" width="9" style="22"/>
-    <col min="11" max="11" width="18.5" style="22" customWidth="1"/>
-    <col min="12" max="12" width="19.375" style="22" customWidth="1"/>
-    <col min="13" max="13" width="20.375" style="22" customWidth="1"/>
-    <col min="14" max="14" width="9" style="22"/>
-    <col min="15" max="15" width="25.75" style="22" customWidth="1"/>
-    <col min="16" max="16" width="16.875" style="22" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="22"/>
+    <col min="10" max="10" width="9.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="22"/>
+    <col min="12" max="12" width="18.5" style="22" customWidth="1"/>
+    <col min="13" max="13" width="19.375" style="22" customWidth="1"/>
+    <col min="14" max="14" width="20.375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="9" style="22"/>
+    <col min="16" max="16" width="25.75" style="22" customWidth="1"/>
+    <col min="17" max="17" width="16.875" style="22" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="42" t="s">
         <v>15</v>
       </c>
@@ -1865,7 +2143,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="41" t="s">
         <v>20</v>
@@ -1873,46 +2151,47 @@
       <c r="J2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="41" t="s">
-        <v>40</v>
-      </c>
+      <c r="K2" s="41"/>
       <c r="L2" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="43" t="s">
+    </row>
+    <row r="3" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="38" t="s">
+      <c r="D3" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>23</v>
-      </c>
       <c r="F3" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="I3" s="40">
         <v>43696</v>
@@ -1920,46 +2199,49 @@
       <c r="J3" s="40">
         <v>43696</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="50">
+        <v>3</v>
+      </c>
+      <c r="L3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="M3" s="26" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="N3" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>63</v>
-      </c>
       <c r="F4" s="24" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="25">
         <v>43696</v>
@@ -1967,46 +2249,49 @@
       <c r="J4" s="25">
         <v>43696</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="M4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="O4" s="29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>31</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I5" s="36">
         <v>43696</v>
@@ -2014,46 +2299,49 @@
       <c r="J5" s="36">
         <v>43696</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="35" t="s">
-        <v>43</v>
-      </c>
       <c r="M5" s="35" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="N5" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="38" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="C6" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="35" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>35</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I6" s="36">
         <v>43696</v>
@@ -2061,116 +2349,666 @@
       <c r="J6" s="36">
         <v>43696</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="L6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="35" t="s">
-        <v>43</v>
-      </c>
       <c r="M6" s="35" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="N6" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="O6" s="37" t="s">
+    </row>
+    <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J7" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K7" s="24">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J8" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="P8" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J9" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K9" s="24">
+        <v>0</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="P9" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="30" t="s">
+      <c r="C10" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J10" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K10" s="24">
+        <v>1</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J11" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K11" s="24">
+        <v>1</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J12" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K12" s="24">
+        <v>1</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J13" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K13" s="24">
+        <v>2</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O13" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J14" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K14" s="24">
+        <v>2</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O14" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="31" t="s">
+      <c r="D15" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J15" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K15" s="24">
+        <v>2</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="P15" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J16" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K16" s="24">
+        <v>3</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="P16" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="R16" s="23"/>
+    </row>
+    <row r="17" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="32">
-        <v>43696</v>
-      </c>
-      <c r="J7" s="32">
-        <v>43696</v>
-      </c>
-      <c r="K7" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="31" t="s">
+      <c r="H17" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="33" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q14" s="23"/>
-    </row>
-    <row r="15" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q15" s="23"/>
-    </row>
-    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q16" s="23"/>
-    </row>
-    <row r="17" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q17" s="23"/>
-    </row>
-    <row r="19" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q19" s="23"/>
-    </row>
-    <row r="20" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q20" s="23"/>
-    </row>
-    <row r="21" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q21" s="23"/>
-    </row>
-    <row r="22" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q22" s="23"/>
-    </row>
-    <row r="30" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O30" s="23"/>
-    </row>
-    <row r="31" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O31" s="23"/>
-    </row>
-    <row r="32" spans="15:17" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O32" s="23"/>
-    </row>
-    <row r="33" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O33" s="23"/>
-    </row>
-    <row r="35" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O35" s="23"/>
-    </row>
-    <row r="36" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O36" s="23"/>
-    </row>
-    <row r="37" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O37" s="23"/>
-    </row>
-    <row r="38" spans="15:15" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O38" s="23"/>
+      <c r="I17" s="25">
+        <v>43697</v>
+      </c>
+      <c r="J17" s="25">
+        <v>43697</v>
+      </c>
+      <c r="K17" s="24">
+        <v>3</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="P17" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="R17" s="23"/>
+    </row>
+    <row r="18" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="32">
+        <v>43697</v>
+      </c>
+      <c r="J18" s="32">
+        <v>43697</v>
+      </c>
+      <c r="K18" s="31">
+        <v>3</v>
+      </c>
+      <c r="L18" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="P18" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="R18" s="23"/>
+    </row>
+    <row r="19" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R19" s="23"/>
+    </row>
+    <row r="21" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R21" s="23"/>
+    </row>
+    <row r="22" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R22" s="23"/>
+    </row>
+    <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R23" s="23"/>
+    </row>
+    <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="R24" s="23"/>
+    </row>
+    <row r="32" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P32" s="23"/>
+    </row>
+    <row r="33" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P33" s="23"/>
+    </row>
+    <row r="34" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P34" s="23"/>
+    </row>
+    <row r="35" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P35" s="23"/>
+    </row>
+    <row r="37" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P37" s="23"/>
+    </row>
+    <row r="38" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P38" s="23"/>
+    </row>
+    <row r="39" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P39" s="23"/>
+    </row>
+    <row r="40" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P40" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2183,7 +3021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EF3A77-BB80-4E84-8A01-F8C91F1840A5}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="P23" sqref="P22:P23"/>
     </sheetView>
   </sheetViews>
@@ -2191,42 +3029,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B9" s="47" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
@@ -2235,7 +3073,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B10" s="49" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="48"/>
@@ -2244,7 +3082,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finit le mongodb pour le get faire le post
</commit_message>
<xml_diff>
--- a/Cahier des charges/READ ME.xlsx
+++ b/Cahier des charges/READ ME.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E18E16-BD25-4DEF-8E01-F3C0AC8E2D38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF4B254-3C04-4D04-8EF7-721F5D7664FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="1" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
   </bookViews>
@@ -2099,7 +2099,7 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
ENFIN FAIT UN BO PROGRAMME!! Ca fait plaisir bande de reported de gens ! Link_models est fonctionel maintenant Reste a finir les finissions !
</commit_message>
<xml_diff>
--- a/Cahier des charges/READ ME.xlsx
+++ b/Cahier des charges/READ ME.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF4B254-3C04-4D04-8EF7-721F5D7664FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20D1E4B-5DD0-435F-B304-3996DDBBDF2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="1" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" firstSheet="1" activeTab="1" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
   </bookViews>
   <sheets>
     <sheet name="ports" sheetId="1" r:id="rId1"/>
-    <sheet name="authentication db info" sheetId="2" r:id="rId2"/>
-    <sheet name="Comment gerer les jwt" sheetId="3" r:id="rId3"/>
+    <sheet name="used database recap" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="authentication db info" sheetId="2" r:id="rId4"/>
+    <sheet name="Comment gerer les jwt" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="119">
   <si>
     <t>Recap des ports used dans les applis node.js</t>
     <phoneticPr fontId="1"/>
@@ -239,10 +241,6 @@
   </si>
   <si>
     <t>live_info</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5a407513b2bc34880b3933</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -412,89 +410,23 @@
     <t>r/rw</t>
   </si>
   <si>
-    <t>KM_db_c1r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c1rw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c2r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c2rw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c3r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c3rw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c1w</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c2w</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c3w</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>access_db_c1r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>access_db_c1w</t>
-  </si>
-  <si>
     <t>access_db_c1rw</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>access_c1r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>access_c1w</t>
-  </si>
-  <si>
     <t>access_c1rw</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>access_c3w</t>
-  </si>
-  <si>
     <t>access_c3rw</t>
   </si>
   <si>
-    <t>access_db_c2w</t>
-  </si>
-  <si>
     <t>access_db_c2rw</t>
   </si>
   <si>
-    <t>access_db_c3w</t>
-  </si>
-  <si>
     <t>access_db_c3rw</t>
   </si>
   <si>
-    <t>access_c2w</t>
-  </si>
-  <si>
     <t>WQ?~&gt;R4z</t>
   </si>
   <si>
@@ -507,27 +439,12 @@
     <t>w4#7Ec$W</t>
   </si>
   <si>
-    <t>GYb!Q52E</t>
-  </si>
-  <si>
     <t>xN!SJ26N</t>
   </si>
   <si>
-    <t>a%66#KFg</t>
-  </si>
-  <si>
-    <t>8P5!J#HL</t>
-  </si>
-  <si>
     <t>&amp;MB3gZBS</t>
   </si>
   <si>
-    <t>+y&amp;WXY@2</t>
-  </si>
-  <si>
-    <t>LJN+Sb59</t>
-  </si>
-  <si>
     <t>uWL845@#</t>
   </si>
   <si>
@@ -563,22 +480,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>B4g+D85Q</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>HTRG%M68</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>!6Dq%h@u</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5b89bcf3f2d3273ce26bd4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>GaDS9?&amp;G</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -587,17 +488,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>access_c2r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>access_db_c2r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5b8a40f3f2d3273ce26bd6</t>
-  </si>
-  <si>
     <t>access_c2rw</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -609,93 +499,24 @@
     <t>5d5b8adbf3f2d3273ce26bd7</t>
   </si>
   <si>
-    <t>nUT+Ds28</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5b8b0df3f2d3273ce26bd8</t>
-  </si>
-  <si>
-    <t>access_c3r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>access_db_c3r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>78B34B^Y</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>LHE?w4Tu</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5b8b32f3f2d3273ce26bd9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>83Lt&amp;^44</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>5d5b8b52f3f2d3273ce26bda</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>5d5b8b69f3f2d3273ce26bdb</t>
   </si>
   <si>
-    <t>6+qx&gt;3R#</t>
-  </si>
-  <si>
-    <t>Q6G&amp;ntmJ</t>
-  </si>
-  <si>
     <t>MXL8D?8k</t>
   </si>
   <si>
-    <t>KM_db_c0r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c0w</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_db_c0rw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>access_c0r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>access_c0w</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>access_c0rw</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>access_db_c0r</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>access_db_c0w</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>access_db_c0rw</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Gf7@SEr7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>eD8D2Ty?</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -703,21 +524,92 @@
     <t>5d5b8fa4a2a3ec5288524f8c</t>
   </si>
   <si>
-    <t>5d5b8fd1a2a3ec5288524f8d</t>
-  </si>
-  <si>
-    <t>UnpD$6CH</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>5d5b8fe6a2a3ec5288524f8e</t>
+    <t xml:space="preserve">Project name </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ajax_db</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>database used</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>filename</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ALL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MongoDbUnitOfWork.js
+MySqlUnitOfWork.js
+UnitOfWorkFactory.js</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jwtGenerator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jwt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>models\authModel.js</t>
+  </si>
+  <si>
+    <t>jwtManager</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>link_tracker</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>link_tracker\tracker.js</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tracker-&gt;CRUD-MYSQL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C:\Workspace\MyEnv\NodeJs\rest\models\GraphApi.js</t>
+  </si>
+  <si>
+    <t>rest</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>models\GraphApi.js,
+models\TrackingApi.js</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mysql_crud</t>
+  </si>
+  <si>
+    <t>mongo_jwt</t>
+  </si>
+  <si>
+    <t>mongo_crud</t>
+  </si>
+  <si>
+    <t>mock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,8 +722,16 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -886,6 +786,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -1162,7 +1068,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1332,6 +1238,45 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1927,7 +1872,7 @@
   <dimension ref="E2:T45"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F5" sqref="F5:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2095,11 +2040,124 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F177E1E-E26F-42A9-BA01-DE66E5CDE2B6}">
+  <dimension ref="B2:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="63.25" customWidth="1"/>
+    <col min="4" max="4" width="29.75" customWidth="1"/>
+    <col min="5" max="5" width="34.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="B4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B6" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="68" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B7" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7B2091-4D89-4C79-A7F9-ACF6A4CE4C20}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1AC559-EAEB-434C-971F-21A81182D7FD}">
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2170,16 +2228,16 @@
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="38" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>22</v>
@@ -2220,16 +2278,16 @@
     </row>
     <row r="4" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="38" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>50</v>
@@ -2250,7 +2308,7 @@
         <v>43696</v>
       </c>
       <c r="K4" s="51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>10</v>
@@ -2270,16 +2328,16 @@
     </row>
     <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="38" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>28</v>
@@ -2300,7 +2358,7 @@
         <v>43696</v>
       </c>
       <c r="K5" s="52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L5" s="35" t="s">
         <v>11</v>
@@ -2320,16 +2378,16 @@
     </row>
     <row r="6" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="38" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>31</v>
@@ -2350,7 +2408,7 @@
         <v>43696</v>
       </c>
       <c r="K6" s="52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L6" s="35" t="s">
         <v>12</v>
@@ -2370,22 +2428,22 @@
     </row>
     <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="55" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="G7" s="24" t="s">
         <v>14</v>
@@ -2412,30 +2470,30 @@
         <v>36</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="P7" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="55" t="s">
-        <v>148</v>
+      <c r="A8" s="53" t="s">
+        <v>86</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>149</v>
+        <v>87</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>133</v>
+        <v>117</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>75</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>142</v>
+        <v>66</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>14</v>
@@ -2450,10 +2508,10 @@
         <v>43697</v>
       </c>
       <c r="K8" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M8" s="24" t="s">
         <v>36</v>
@@ -2462,30 +2520,30 @@
         <v>36</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="P8" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="55" t="s">
-        <v>145</v>
+      <c r="A9" s="54" t="s">
+        <v>89</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>146</v>
+        <v>90</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" s="56" t="s">
-        <v>134</v>
+        <v>116</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>76</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="G9" s="24" t="s">
         <v>14</v>
@@ -2500,10 +2558,10 @@
         <v>43697</v>
       </c>
       <c r="K9" s="24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="M9" s="24" t="s">
         <v>36</v>
@@ -2512,503 +2570,101 @@
         <v>36</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P9" s="29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="24" t="s">
+    <row r="10" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="E10" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="32">
         <v>43697</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="32">
         <v>43697</v>
       </c>
-      <c r="K10" s="24">
-        <v>1</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="24" t="s">
+      <c r="K10" s="31">
+        <v>3</v>
+      </c>
+      <c r="L10" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="M10" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="P10" s="29" t="s">
+      <c r="N10" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="33" t="s">
         <v>45</v>
       </c>
+      <c r="R10" s="23"/>
     </row>
     <row r="11" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="53" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="25">
-        <v>43697</v>
-      </c>
-      <c r="J11" s="25">
-        <v>43697</v>
-      </c>
-      <c r="K11" s="24">
-        <v>1</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O11" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="P11" s="29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="25">
-        <v>43697</v>
-      </c>
-      <c r="J12" s="25">
-        <v>43697</v>
-      </c>
-      <c r="K12" s="24">
-        <v>1</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O12" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="P12" s="29" t="s">
-        <v>45</v>
-      </c>
+      <c r="R11" s="23"/>
     </row>
     <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="54" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="25">
-        <v>43697</v>
-      </c>
-      <c r="J13" s="25">
-        <v>43697</v>
-      </c>
-      <c r="K13" s="24">
-        <v>2</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O13" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="P13" s="29" t="s">
-        <v>45</v>
-      </c>
+      <c r="R13" s="23"/>
     </row>
     <row r="14" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I14" s="25">
-        <v>43697</v>
-      </c>
-      <c r="J14" s="25">
-        <v>43697</v>
-      </c>
-      <c r="K14" s="24">
-        <v>2</v>
-      </c>
-      <c r="L14" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O14" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="P14" s="29" t="s">
-        <v>45</v>
-      </c>
+      <c r="R14" s="23"/>
     </row>
     <row r="15" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="25">
-        <v>43697</v>
-      </c>
-      <c r="J15" s="25">
-        <v>43697</v>
-      </c>
-      <c r="K15" s="24">
-        <v>2</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N15" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O15" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="P15" s="29" t="s">
-        <v>45</v>
-      </c>
+      <c r="R15" s="23"/>
     </row>
     <row r="16" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I16" s="25">
-        <v>43697</v>
-      </c>
-      <c r="J16" s="25">
-        <v>43697</v>
-      </c>
-      <c r="K16" s="24">
-        <v>3</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="M16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O16" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="P16" s="29" t="s">
-        <v>45</v>
-      </c>
       <c r="R16" s="23"/>
     </row>
-    <row r="17" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="25">
-        <v>43697</v>
-      </c>
-      <c r="J17" s="25">
-        <v>43697</v>
-      </c>
-      <c r="K17" s="24">
-        <v>3</v>
-      </c>
-      <c r="L17" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O17" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="P17" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="R17" s="23"/>
-    </row>
-    <row r="18" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="32">
-        <v>43697</v>
-      </c>
-      <c r="J18" s="32">
-        <v>43697</v>
-      </c>
-      <c r="K18" s="31">
-        <v>3</v>
-      </c>
-      <c r="L18" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="M18" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="N18" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="O18" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="P18" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="R18" s="23"/>
-    </row>
-    <row r="19" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="R19" s="23"/>
-    </row>
-    <row r="21" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="R21" s="23"/>
-    </row>
-    <row r="22" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="R22" s="23"/>
-    </row>
-    <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="R23" s="23"/>
-    </row>
-    <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="R24" s="23"/>
-    </row>
-    <row r="32" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P24" s="23"/>
+    </row>
+    <row r="25" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P25" s="23"/>
+    </row>
+    <row r="26" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P26" s="23"/>
+    </row>
+    <row r="27" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P27" s="23"/>
+    </row>
+    <row r="29" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P29" s="23"/>
+    </row>
+    <row r="30" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P30" s="23"/>
+    </row>
+    <row r="31" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="P31" s="23"/>
+    </row>
+    <row r="32" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="P32" s="23"/>
-    </row>
-    <row r="33" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="P33" s="23"/>
-    </row>
-    <row r="34" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="P34" s="23"/>
-    </row>
-    <row r="35" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="P35" s="23"/>
-    </row>
-    <row r="37" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="P37" s="23"/>
-    </row>
-    <row r="38" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="P38" s="23"/>
-    </row>
-    <row r="39" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="P39" s="23"/>
-    </row>
-    <row r="40" spans="16:16" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="P40" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -3017,7 +2673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EF3A77-BB80-4E84-8A01-F8C91F1840A5}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -3029,42 +2685,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B9" s="47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
@@ -3073,7 +2729,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B10" s="49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="48"/>
@@ -3082,7 +2738,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finis le logging avance travail sur les error
</commit_message>
<xml_diff>
--- a/Cahier des charges/READ ME.xlsx
+++ b/Cahier des charges/READ ME.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEC7E4D-D3FD-4E22-B2C6-3F83FC78D4CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3FA03F-8F1D-4584-AAE3-5DACAFB9C2AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="1" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="146">
   <si>
     <t>Recap des ports used dans les applis node.js</t>
     <phoneticPr fontId="1"/>
@@ -2356,7 +2356,7 @@
   <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2462,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7B2091-4D89-4C79-A7F9-ACF6A4CE4C20}">
   <dimension ref="C1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
link_http_code terminer gestion des erreur termine Check all request ajax termine!
</commit_message>
<xml_diff>
--- a/Cahier des charges/READ ME.xlsx
+++ b/Cahier des charges/READ ME.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3FA03F-8F1D-4584-AAE3-5DACAFB9C2AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE978D8-4689-4471-9A62-B4544E64B28A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="1" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="3" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
   </bookViews>
   <sheets>
     <sheet name="ports" sheetId="1" r:id="rId1"/>
@@ -2355,8 +2355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F177E1E-E26F-42A9-BA01-DE66E5CDE2B6}">
   <dimension ref="B2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2463,7 +2463,7 @@
   <dimension ref="C1:E13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2606,8 +2606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1AC559-EAEB-434C-971F-21A81182D7FD}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Grosse Update avec Last Version de Galaxy Breaker
</commit_message>
<xml_diff>
--- a/Cahier des charges/READ ME.xlsx
+++ b/Cahier des charges/READ ME.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyEnv\NodeJs\Cahier des charges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE978D8-4689-4471-9A62-B4544E64B28A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CCAF08-9E61-4744-991A-8DDE396BD33D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7395" activeTab="3" xr2:uid="{374B1BF0-F420-49F4-96B0-4DC0BCC3FEC3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="147">
   <si>
     <t>Recap des ports used dans les applis node.js</t>
     <phoneticPr fontId="1"/>
@@ -141,18 +141,6 @@
   </si>
   <si>
     <t>KM_graph</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KM_Bejewel</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bejewel</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>game1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -712,12 +700,37 @@
     <t>ok</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>KM_GalaxyBreaker</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Galaxy_Breaker</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>galaxy_breaker</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>まだ</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,6 +843,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1281,7 +1301,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1550,6 +1570,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2241,7 +2267,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="5:7" ht="75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2370,13 +2396,13 @@
     <row r="2" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="89" t="s">
         <v>98</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="89" t="s">
-        <v>101</v>
       </c>
       <c r="E3" s="88">
         <v>43707</v>
@@ -2384,72 +2410,72 @@
     </row>
     <row r="4" spans="2:5" ht="56.25" x14ac:dyDescent="0.4">
       <c r="B4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="D4" s="78" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E4" s="83" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E5" s="84" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B6" s="58" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E6" s="85" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B7" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E7" s="86" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="59" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C8" s="60" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D8" s="82" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E8" s="87" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2462,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D7B2091-4D89-4C79-A7F9-ACF6A4CE4C20}">
   <dimension ref="C1:E13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2475,21 +2501,21 @@
     <row r="1" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C3" s="75" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E3" s="77">
         <v>3002</v>
@@ -2497,10 +2523,10 @@
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C4" s="65" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E4" s="66">
         <v>3000</v>
@@ -2508,10 +2534,10 @@
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C5" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E5" s="18">
         <v>3001</v>
@@ -2519,10 +2545,10 @@
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C6" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E6" s="9">
         <v>3003</v>
@@ -2530,10 +2556,10 @@
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C7" s="67" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E7" s="68">
         <v>3004</v>
@@ -2541,58 +2567,58 @@
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C8" s="69" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E8" s="70"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C9" s="71" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E9" s="70"/>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C10" s="69" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E10" s="70"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C11" s="69" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E11" s="70"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C12" s="71" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E12" s="70"/>
     </row>
     <row r="13" spans="3:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C13" s="72" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D13" s="73" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E13" s="74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2607,7 +2633,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:P2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2661,33 +2687,33 @@
       </c>
       <c r="K2" s="41"/>
       <c r="L2" s="41" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M2" s="41" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N2" s="41" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O2" s="41" t="s">
         <v>8</v>
       </c>
       <c r="P2" s="43" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>22</v>
@@ -2699,7 +2725,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I3" s="40">
         <v>43696</v>
@@ -2714,36 +2740,36 @@
         <v>9</v>
       </c>
       <c r="M3" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N3" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O3" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P3" s="27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="38" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>14</v>
@@ -2758,98 +2784,98 @@
         <v>43696</v>
       </c>
       <c r="K4" s="51" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P4" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="36">
-        <v>43696</v>
-      </c>
-      <c r="J5" s="36">
-        <v>43696</v>
-      </c>
-      <c r="K5" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" s="35" t="s">
+      <c r="H5" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="25">
+        <v>43857</v>
+      </c>
+      <c r="J5" s="25">
+        <v>43857</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="O5" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="37" t="s">
-        <v>44</v>
+      <c r="M5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="29" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I6" s="36">
         <v>43696</v>
@@ -2858,48 +2884,48 @@
         <v>43696</v>
       </c>
       <c r="K6" s="52" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L6" s="35" t="s">
         <v>12</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N6" s="35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O6" s="35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="P6" s="37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="55" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G7" s="24" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I7" s="25">
         <v>43697</v>
@@ -2911,45 +2937,45 @@
         <v>0</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P7" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="53" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I8" s="25">
         <v>43697</v>
@@ -2961,45 +2987,45 @@
         <v>1</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P8" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="54" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G9" s="24" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I9" s="25">
         <v>43697</v>
@@ -3014,42 +3040,42 @@
         <v>9</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P9" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="54" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I10" s="32">
         <v>43697</v>
@@ -3061,19 +3087,19 @@
         <v>3</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M10" s="31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O10" s="31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P10" s="33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R10" s="23"/>
     </row>
@@ -3135,42 +3161,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B9" s="47" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
@@ -3179,7 +3205,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B10" s="49" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="48"/>
@@ -3188,7 +3214,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>